<commit_message>
Updated the rest of the test config files and excel spreadsheets
</commit_message>
<xml_diff>
--- a/tests/Feature/config/house_zero.xlsx
+++ b/tests/Feature/config/house_zero.xlsx
@@ -112,7 +112,7 @@
     <t>Anskaffelsesverdi</t>
   </si>
   <si>
-    <t>Betalt (inkl kostnader)</t>
+    <t>Finans kostnader)</t>
   </si>
   <si>
     <t>Skattbar</t>
@@ -151,13 +151,13 @@
     <t>Here I live</t>
   </si>
   <si>
-    <t xml:space="preserve">000 Asset rule </t>
+    <t xml:space="preserve"> Asset rule: </t>
   </si>
   <si>
-    <t>0Kommunale/Forsikring/Strøm/Eiendomsskatt 7300 mnd Asset rule Using current amount: 3000000 * 1</t>
+    <t>Kommunale/Forsikring/Strøm/Eiendomsskatt 7300 mnd Asset rule: Using current amount: 3000000 * 1</t>
   </si>
   <si>
-    <t>000 Asset rule Using current amount: 3000000 * 1</t>
+    <t xml:space="preserve"> Asset rule: Using current amount: 3000000 * 1</t>
   </si>
   <si>
     <t>total</t>
@@ -573,16 +573,16 @@
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="37.705" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="6.998" bestFit="true" customWidth="true" style="0"/>
@@ -1684,17 +1684,17 @@
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="1">
-        <v>0</v>
+        <v>15000.0</v>
       </c>
       <c r="L18" s="1">
-        <v>0</v>
+        <v>68123.0</v>
       </c>
       <c r="M18" s="1">
-        <v>0</v>
+        <v>1431877.0</v>
       </c>
       <c r="N18" s="1">
         <v>0</v>
@@ -1705,13 +1705,13 @@
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="1">
-        <v>3000000.0</v>
+        <v>1568123.0</v>
       </c>
       <c r="S18" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T18" s="1">
-        <v>3000000.0</v>
+        <v>1500000.0</v>
       </c>
       <c r="U18" s="6">
         <v>750000.0</v>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="1">
@@ -1738,6 +1738,9 @@
         <v>0.0</v>
       </c>
       <c r="AE18"/>
+      <c r="AF18">
+        <v>0</v>
+      </c>
       <c r="AG18"/>
     </row>
     <row r="19" spans="1:33">
@@ -1760,17 +1763,17 @@
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="8">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="8">
-        <v>0</v>
+        <v>14319.0</v>
       </c>
       <c r="L19" s="8">
-        <v>0</v>
+        <v>68804.0</v>
       </c>
       <c r="M19" s="8">
-        <v>0</v>
+        <v>1363073.0</v>
       </c>
       <c r="N19" s="8">
         <v>0</v>
@@ -1781,13 +1784,13 @@
       </c>
       <c r="Q19" s="9"/>
       <c r="R19" s="8">
-        <v>3000000.0</v>
+        <v>1636927.0</v>
       </c>
       <c r="S19" s="8">
         <v>3000000.0</v>
       </c>
       <c r="T19" s="8">
-        <v>3000000.0</v>
+        <v>1583123.0</v>
       </c>
       <c r="U19" s="8">
         <v>750000.0</v>
@@ -1798,7 +1801,7 @@
       </c>
       <c r="X19" s="9"/>
       <c r="Y19" s="8">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z19" s="9"/>
       <c r="AA19" s="8">
@@ -1814,7 +1817,9 @@
         <v>0.0</v>
       </c>
       <c r="AE19" s="7"/>
-      <c r="AF19" s="7"/>
+      <c r="AF19" s="7">
+        <v>0</v>
+      </c>
       <c r="AG19"/>
     </row>
     <row r="20" spans="1:33">
@@ -1837,17 +1842,17 @@
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="1">
-        <v>0</v>
+        <v>13631.0</v>
       </c>
       <c r="L20" s="1">
-        <v>0</v>
+        <v>69492.0</v>
       </c>
       <c r="M20" s="1">
-        <v>0</v>
+        <v>1293581.0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
@@ -1858,13 +1863,13 @@
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="1">
-        <v>3000000.0</v>
+        <v>1706419.0</v>
       </c>
       <c r="S20" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T20" s="1">
-        <v>3000000.0</v>
+        <v>1666246.0</v>
       </c>
       <c r="U20" s="6">
         <v>750000.0</v>
@@ -1875,7 +1880,7 @@
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
@@ -1891,6 +1896,9 @@
         <v>0.0</v>
       </c>
       <c r="AE20"/>
+      <c r="AF20">
+        <v>0</v>
+      </c>
       <c r="AG20"/>
     </row>
     <row r="21" spans="1:33">
@@ -1913,17 +1921,17 @@
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="1">
-        <v>0</v>
+        <v>12936.0</v>
       </c>
       <c r="L21" s="1">
-        <v>0</v>
+        <v>70187.0</v>
       </c>
       <c r="M21" s="1">
-        <v>0</v>
+        <v>1223393.0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
@@ -1934,13 +1942,13 @@
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="1">
-        <v>3000000.0</v>
+        <v>1776607.0</v>
       </c>
       <c r="S21" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T21" s="1">
-        <v>3000000.0</v>
+        <v>1749369.0</v>
       </c>
       <c r="U21" s="6">
         <v>750000.0</v>
@@ -1951,7 +1959,7 @@
       </c>
       <c r="X21" s="2"/>
       <c r="Y21" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="1">
@@ -1967,6 +1975,9 @@
         <v>0.0</v>
       </c>
       <c r="AE21"/>
+      <c r="AF21">
+        <v>0</v>
+      </c>
       <c r="AG21"/>
     </row>
     <row r="22" spans="1:33">
@@ -1989,17 +2000,17 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="1">
-        <v>0</v>
+        <v>12234.0</v>
       </c>
       <c r="L22" s="1">
-        <v>0</v>
+        <v>70889.0</v>
       </c>
       <c r="M22" s="1">
-        <v>0</v>
+        <v>1152504.0</v>
       </c>
       <c r="N22" s="1">
         <v>0</v>
@@ -2010,13 +2021,13 @@
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="1">
-        <v>3000000.0</v>
+        <v>1847496.0</v>
       </c>
       <c r="S22" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T22" s="1">
-        <v>3000000.0</v>
+        <v>1832492.0</v>
       </c>
       <c r="U22" s="6">
         <v>750000.0</v>
@@ -2027,7 +2038,7 @@
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="1">
@@ -2043,6 +2054,9 @@
         <v>0.0</v>
       </c>
       <c r="AE22"/>
+      <c r="AF22">
+        <v>0</v>
+      </c>
       <c r="AG22"/>
     </row>
     <row r="23" spans="1:33">
@@ -2065,17 +2079,17 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="1">
-        <v>0</v>
+        <v>11525.0</v>
       </c>
       <c r="L23" s="1">
-        <v>0</v>
+        <v>71598.0</v>
       </c>
       <c r="M23" s="1">
-        <v>0</v>
+        <v>1080906.0</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
@@ -2086,13 +2100,13 @@
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="1">
-        <v>3000000.0</v>
+        <v>1919094.0</v>
       </c>
       <c r="S23" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T23" s="1">
-        <v>3000000.0</v>
+        <v>1915615.0</v>
       </c>
       <c r="U23" s="6">
         <v>750000.0</v>
@@ -2103,7 +2117,7 @@
       </c>
       <c r="X23" s="2"/>
       <c r="Y23" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="1">
@@ -2119,6 +2133,9 @@
         <v>0.0</v>
       </c>
       <c r="AE23"/>
+      <c r="AF23">
+        <v>0</v>
+      </c>
       <c r="AG23"/>
     </row>
     <row r="24" spans="1:33">
@@ -2141,17 +2158,17 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="1">
-        <v>0</v>
+        <v>10809.0</v>
       </c>
       <c r="L24" s="1">
-        <v>0</v>
+        <v>72314.0</v>
       </c>
       <c r="M24" s="1">
-        <v>0</v>
+        <v>1008593.0</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
@@ -2162,13 +2179,13 @@
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="1">
-        <v>3000000.0</v>
+        <v>1991407.0</v>
       </c>
       <c r="S24" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T24" s="1">
-        <v>3000000.0</v>
+        <v>1998738.0</v>
       </c>
       <c r="U24" s="6">
         <v>750000.0</v>
@@ -2179,7 +2196,7 @@
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="1">
@@ -2195,6 +2212,9 @@
         <v>0.0</v>
       </c>
       <c r="AE24"/>
+      <c r="AF24">
+        <v>0</v>
+      </c>
       <c r="AG24"/>
     </row>
     <row r="25" spans="1:33">
@@ -2217,17 +2237,17 @@
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="1">
-        <v>0</v>
+        <v>10086.0</v>
       </c>
       <c r="L25" s="1">
-        <v>0</v>
+        <v>73037.0</v>
       </c>
       <c r="M25" s="1">
-        <v>0</v>
+        <v>935555.0</v>
       </c>
       <c r="N25" s="1">
         <v>0</v>
@@ -2238,13 +2258,13 @@
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="1">
-        <v>3000000.0</v>
+        <v>2064445.0</v>
       </c>
       <c r="S25" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T25" s="1">
-        <v>3000000.0</v>
+        <v>2081861.0</v>
       </c>
       <c r="U25" s="6">
         <v>750000.0</v>
@@ -2255,7 +2275,7 @@
       </c>
       <c r="X25" s="2"/>
       <c r="Y25" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z25" s="2"/>
       <c r="AA25" s="1">
@@ -2271,6 +2291,9 @@
         <v>0.0</v>
       </c>
       <c r="AE25"/>
+      <c r="AF25">
+        <v>0</v>
+      </c>
       <c r="AG25"/>
     </row>
     <row r="26" spans="1:33">
@@ -2293,17 +2316,17 @@
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="1">
-        <v>0</v>
+        <v>9356.0</v>
       </c>
       <c r="L26" s="1">
-        <v>0</v>
+        <v>73767.0</v>
       </c>
       <c r="M26" s="1">
-        <v>0</v>
+        <v>861788.0</v>
       </c>
       <c r="N26" s="1">
         <v>0</v>
@@ -2314,13 +2337,13 @@
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="1">
-        <v>3000000.0</v>
+        <v>2138212.0</v>
       </c>
       <c r="S26" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T26" s="1">
-        <v>3000000.0</v>
+        <v>2164984.0</v>
       </c>
       <c r="U26" s="6">
         <v>750000.0</v>
@@ -2331,7 +2354,7 @@
       </c>
       <c r="X26" s="2"/>
       <c r="Y26" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="1">
@@ -2347,6 +2370,9 @@
         <v>0.0</v>
       </c>
       <c r="AE26"/>
+      <c r="AF26">
+        <v>0</v>
+      </c>
       <c r="AG26"/>
     </row>
     <row r="27" spans="1:33">
@@ -2369,17 +2395,17 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="1">
-        <v>0</v>
+        <v>8618.0</v>
       </c>
       <c r="L27" s="1">
-        <v>0</v>
+        <v>74505.0</v>
       </c>
       <c r="M27" s="1">
-        <v>0</v>
+        <v>787283.0</v>
       </c>
       <c r="N27" s="1">
         <v>0</v>
@@ -2390,13 +2416,13 @@
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="1">
-        <v>3000000.0</v>
+        <v>2212717.0</v>
       </c>
       <c r="S27" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T27" s="1">
-        <v>3000000.0</v>
+        <v>2248107.0</v>
       </c>
       <c r="U27" s="6">
         <v>750000.0</v>
@@ -2407,7 +2433,7 @@
       </c>
       <c r="X27" s="2"/>
       <c r="Y27" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="1">
@@ -2423,6 +2449,9 @@
         <v>0.0</v>
       </c>
       <c r="AE27"/>
+      <c r="AF27">
+        <v>0</v>
+      </c>
       <c r="AG27"/>
     </row>
     <row r="28" spans="1:33">
@@ -2445,17 +2474,17 @@
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="1">
-        <v>0</v>
+        <v>7873.0</v>
       </c>
       <c r="L28" s="1">
-        <v>0</v>
+        <v>75250.0</v>
       </c>
       <c r="M28" s="1">
-        <v>0</v>
+        <v>712033.0</v>
       </c>
       <c r="N28" s="1">
         <v>0</v>
@@ -2466,13 +2495,13 @@
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="1">
-        <v>3000000.0</v>
+        <v>2287967.0</v>
       </c>
       <c r="S28" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T28" s="1">
-        <v>3000000.0</v>
+        <v>2331230.0</v>
       </c>
       <c r="U28" s="6">
         <v>750000.0</v>
@@ -2483,7 +2512,7 @@
       </c>
       <c r="X28" s="2"/>
       <c r="Y28" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="1">
@@ -2499,6 +2528,9 @@
         <v>0.0</v>
       </c>
       <c r="AE28"/>
+      <c r="AF28">
+        <v>0</v>
+      </c>
       <c r="AG28"/>
     </row>
     <row r="29" spans="1:33">
@@ -2521,17 +2553,17 @@
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="1">
-        <v>0</v>
+        <v>7120.0</v>
       </c>
       <c r="L29" s="1">
-        <v>0</v>
+        <v>76003.0</v>
       </c>
       <c r="M29" s="1">
-        <v>0</v>
+        <v>636030.0</v>
       </c>
       <c r="N29" s="1">
         <v>0</v>
@@ -2542,13 +2574,13 @@
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="1">
-        <v>3000000.0</v>
+        <v>2363970.0</v>
       </c>
       <c r="S29" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T29" s="1">
-        <v>3000000.0</v>
+        <v>2414353.0</v>
       </c>
       <c r="U29" s="6">
         <v>750000.0</v>
@@ -2559,7 +2591,7 @@
       </c>
       <c r="X29" s="2"/>
       <c r="Y29" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="1">
@@ -2575,6 +2607,9 @@
         <v>0.0</v>
       </c>
       <c r="AE29"/>
+      <c r="AF29">
+        <v>0</v>
+      </c>
       <c r="AG29"/>
     </row>
     <row r="30" spans="1:33">
@@ -2597,17 +2632,17 @@
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="1">
-        <v>0</v>
+        <v>6360.0</v>
       </c>
       <c r="L30" s="1">
-        <v>0</v>
+        <v>76763.0</v>
       </c>
       <c r="M30" s="1">
-        <v>0</v>
+        <v>559268.0</v>
       </c>
       <c r="N30" s="1">
         <v>0</v>
@@ -2618,13 +2653,13 @@
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="1">
-        <v>3000000.0</v>
+        <v>2440732.0</v>
       </c>
       <c r="S30" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T30" s="1">
-        <v>3000000.0</v>
+        <v>2497476.0</v>
       </c>
       <c r="U30" s="6">
         <v>750000.0</v>
@@ -2635,7 +2670,7 @@
       </c>
       <c r="X30" s="2"/>
       <c r="Y30" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="1">
@@ -2651,6 +2686,9 @@
         <v>0.0</v>
       </c>
       <c r="AE30"/>
+      <c r="AF30">
+        <v>0</v>
+      </c>
       <c r="AG30"/>
     </row>
     <row r="31" spans="1:33">
@@ -2673,17 +2711,17 @@
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="1">
-        <v>0</v>
+        <v>5593.0</v>
       </c>
       <c r="L31" s="1">
-        <v>0</v>
+        <v>77530.0</v>
       </c>
       <c r="M31" s="1">
-        <v>0</v>
+        <v>481737.0</v>
       </c>
       <c r="N31" s="1">
         <v>0</v>
@@ -2694,13 +2732,13 @@
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="1">
-        <v>3000000.0</v>
+        <v>2518263.0</v>
       </c>
       <c r="S31" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T31" s="1">
-        <v>3000000.0</v>
+        <v>2580599.0</v>
       </c>
       <c r="U31" s="6">
         <v>750000.0</v>
@@ -2711,7 +2749,7 @@
       </c>
       <c r="X31" s="2"/>
       <c r="Y31" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="1">
@@ -2727,6 +2765,9 @@
         <v>0.0</v>
       </c>
       <c r="AE31"/>
+      <c r="AF31">
+        <v>0</v>
+      </c>
       <c r="AG31"/>
     </row>
     <row r="32" spans="1:33">
@@ -2749,17 +2790,17 @@
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="1">
-        <v>0</v>
+        <v>4817.0</v>
       </c>
       <c r="L32" s="1">
-        <v>0</v>
+        <v>78306.0</v>
       </c>
       <c r="M32" s="1">
-        <v>0</v>
+        <v>403432.0</v>
       </c>
       <c r="N32" s="1">
         <v>0</v>
@@ -2770,13 +2811,13 @@
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="1">
-        <v>3000000.0</v>
+        <v>2596568.0</v>
       </c>
       <c r="S32" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T32" s="1">
-        <v>3000000.0</v>
+        <v>2663722.0</v>
       </c>
       <c r="U32" s="6">
         <v>750000.0</v>
@@ -2787,7 +2828,7 @@
       </c>
       <c r="X32" s="2"/>
       <c r="Y32" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="1">
@@ -2803,6 +2844,9 @@
         <v>0.0</v>
       </c>
       <c r="AE32"/>
+      <c r="AF32">
+        <v>0</v>
+      </c>
       <c r="AG32"/>
     </row>
     <row r="33" spans="1:33">
@@ -2825,17 +2869,17 @@
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="1">
-        <v>0</v>
+        <v>4034.0</v>
       </c>
       <c r="L33" s="1">
-        <v>0</v>
+        <v>79089.0</v>
       </c>
       <c r="M33" s="1">
-        <v>0</v>
+        <v>324343.0</v>
       </c>
       <c r="N33" s="1">
         <v>0</v>
@@ -2846,13 +2890,13 @@
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="1">
-        <v>3000000.0</v>
+        <v>2675657.0</v>
       </c>
       <c r="S33" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T33" s="1">
-        <v>3000000.0</v>
+        <v>2746845.0</v>
       </c>
       <c r="U33" s="6">
         <v>750000.0</v>
@@ -2863,7 +2907,7 @@
       </c>
       <c r="X33" s="2"/>
       <c r="Y33" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z33" s="2"/>
       <c r="AA33" s="1">
@@ -2879,6 +2923,9 @@
         <v>0.0</v>
       </c>
       <c r="AE33"/>
+      <c r="AF33">
+        <v>0</v>
+      </c>
       <c r="AG33"/>
     </row>
     <row r="34" spans="1:33">
@@ -2901,17 +2948,17 @@
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="1">
-        <v>0</v>
+        <v>3243.0</v>
       </c>
       <c r="L34" s="1">
-        <v>0</v>
+        <v>79880.0</v>
       </c>
       <c r="M34" s="1">
-        <v>0</v>
+        <v>244463.0</v>
       </c>
       <c r="N34" s="1">
         <v>0</v>
@@ -2922,13 +2969,13 @@
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="1">
-        <v>3000000.0</v>
+        <v>2755537.0</v>
       </c>
       <c r="S34" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T34" s="1">
-        <v>3000000.0</v>
+        <v>2829968.0</v>
       </c>
       <c r="U34" s="6">
         <v>750000.0</v>
@@ -2939,7 +2986,7 @@
       </c>
       <c r="X34" s="2"/>
       <c r="Y34" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="1">
@@ -2955,6 +3002,9 @@
         <v>0.0</v>
       </c>
       <c r="AE34"/>
+      <c r="AF34">
+        <v>0</v>
+      </c>
       <c r="AG34"/>
     </row>
     <row r="35" spans="1:33">
@@ -2977,17 +3027,17 @@
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="1">
-        <v>0</v>
+        <v>2445.0</v>
       </c>
       <c r="L35" s="1">
-        <v>0</v>
+        <v>80678.0</v>
       </c>
       <c r="M35" s="1">
-        <v>0</v>
+        <v>163785.0</v>
       </c>
       <c r="N35" s="1">
         <v>0</v>
@@ -2998,13 +3048,13 @@
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="1">
-        <v>3000000.0</v>
+        <v>2836215.0</v>
       </c>
       <c r="S35" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T35" s="1">
-        <v>3000000.0</v>
+        <v>2913091.0</v>
       </c>
       <c r="U35" s="6">
         <v>750000.0</v>
@@ -3015,7 +3065,7 @@
       </c>
       <c r="X35" s="2"/>
       <c r="Y35" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="1">
@@ -3031,6 +3081,9 @@
         <v>0.0</v>
       </c>
       <c r="AE35"/>
+      <c r="AF35">
+        <v>0</v>
+      </c>
       <c r="AG35"/>
     </row>
     <row r="36" spans="1:33">
@@ -3053,17 +3106,17 @@
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="1">
-        <v>0</v>
+        <v>1638.0</v>
       </c>
       <c r="L36" s="1">
-        <v>0</v>
+        <v>81485.0</v>
       </c>
       <c r="M36" s="1">
-        <v>0</v>
+        <v>82300.0</v>
       </c>
       <c r="N36" s="1">
         <v>0</v>
@@ -3074,13 +3127,13 @@
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="1">
-        <v>3000000.0</v>
+        <v>2917700.0</v>
       </c>
       <c r="S36" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T36" s="1">
-        <v>3000000.0</v>
+        <v>2996214.0</v>
       </c>
       <c r="U36" s="6">
         <v>750000.0</v>
@@ -3091,7 +3144,7 @@
       </c>
       <c r="X36" s="2"/>
       <c r="Y36" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="1">
@@ -3107,6 +3160,9 @@
         <v>0.0</v>
       </c>
       <c r="AE36"/>
+      <c r="AF36">
+        <v>0</v>
+      </c>
       <c r="AG36"/>
     </row>
     <row r="37" spans="1:33">
@@ -3129,17 +3185,17 @@
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="1">
-        <v>0</v>
+        <v>83123.0</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="1">
-        <v>0</v>
+        <v>823.0</v>
       </c>
       <c r="L37" s="1">
-        <v>0</v>
+        <v>82300.0</v>
       </c>
       <c r="M37" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="N37" s="1">
         <v>0</v>
@@ -3156,7 +3212,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T37" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U37" s="6">
         <v>750000.0</v>
@@ -3167,7 +3223,7 @@
       </c>
       <c r="X37" s="2"/>
       <c r="Y37" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="1">
@@ -3183,6 +3239,9 @@
         <v>0.0</v>
       </c>
       <c r="AE37"/>
+      <c r="AF37">
+        <v>0</v>
+      </c>
       <c r="AG37"/>
     </row>
     <row r="38" spans="1:33">
@@ -3232,7 +3291,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T38" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U38" s="6">
         <v>750000.0</v>
@@ -3308,7 +3367,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T39" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U39" s="6">
         <v>750000.0</v>
@@ -3384,7 +3443,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T40" s="11">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U40" s="11">
         <v>750000.0</v>
@@ -3461,7 +3520,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T41" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U41" s="6">
         <v>750000.0</v>
@@ -3537,7 +3596,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T42" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U42" s="6">
         <v>750000.0</v>
@@ -3613,7 +3672,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T43" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U43" s="6">
         <v>750000.0</v>
@@ -3689,7 +3748,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T44" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U44" s="6">
         <v>750000.0</v>
@@ -3765,7 +3824,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T45" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U45" s="6">
         <v>750000.0</v>
@@ -3841,7 +3900,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T46" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U46" s="6">
         <v>750000.0</v>
@@ -3917,7 +3976,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T47" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U47" s="6">
         <v>750000.0</v>
@@ -3993,7 +4052,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T48" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U48" s="6">
         <v>750000.0</v>
@@ -4069,7 +4128,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T49" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U49" s="6">
         <v>750000.0</v>
@@ -4145,7 +4204,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T50" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U50" s="6">
         <v>750000.0</v>
@@ -4221,7 +4280,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T51" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U51" s="6">
         <v>750000.0</v>
@@ -4297,7 +4356,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T52" s="5">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U52" s="5">
         <v>750000.0</v>
@@ -5214,16 +5273,16 @@
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="32.992" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="6.998" bestFit="true" customWidth="true" style="0"/>
@@ -5441,7 +5500,7 @@
       </c>
       <c r="V6" s="2"/>
       <c r="W6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="1">
@@ -5509,7 +5568,7 @@
       </c>
       <c r="V7" s="2"/>
       <c r="W7" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="1">
@@ -5577,7 +5636,7 @@
       </c>
       <c r="V8" s="2"/>
       <c r="W8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="1">
@@ -5645,7 +5704,7 @@
       </c>
       <c r="V9" s="2"/>
       <c r="W9" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="1">
@@ -5713,7 +5772,7 @@
       </c>
       <c r="V10" s="2"/>
       <c r="W10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="1">
@@ -5781,7 +5840,7 @@
       </c>
       <c r="V11" s="2"/>
       <c r="W11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="1">
@@ -5849,7 +5908,7 @@
       </c>
       <c r="V12" s="2"/>
       <c r="W12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="1">
@@ -5917,7 +5976,7 @@
       </c>
       <c r="V13" s="2"/>
       <c r="W13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="1">
@@ -5985,7 +6044,7 @@
       </c>
       <c r="V14" s="2"/>
       <c r="W14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="1">
@@ -6053,7 +6112,7 @@
       </c>
       <c r="V15" s="2"/>
       <c r="W15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="1">
@@ -6121,7 +6180,7 @@
       </c>
       <c r="V16" s="2"/>
       <c r="W16" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="1">
@@ -6189,7 +6248,7 @@
       </c>
       <c r="V17" s="2"/>
       <c r="W17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="1">
@@ -6232,11 +6291,21 @@
         <v>0.0</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="I18" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K18" s="1">
+        <v>15000.0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>68123.0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1431877.0</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="2"/>
       <c r="P18" s="6">
@@ -6244,13 +6313,13 @@
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="1">
-        <v>3000000.0</v>
+        <v>1568123.0</v>
       </c>
       <c r="S18" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T18" s="1">
-        <v>3000000.0</v>
+        <v>1500000.0</v>
       </c>
       <c r="U18" s="6">
         <v>750000.0</v>
@@ -6259,13 +6328,13 @@
         <v>0.25</v>
       </c>
       <c r="W18" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X18" s="2">
         <v>0.01</v>
       </c>
       <c r="Y18" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="1">
@@ -6304,11 +6373,21 @@
         <v>0.0</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="I19" s="8">
+        <v>83123.0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K19" s="8">
+        <v>14319.0</v>
+      </c>
+      <c r="L19" s="8">
+        <v>68804.0</v>
+      </c>
+      <c r="M19" s="8">
+        <v>1363073.0</v>
+      </c>
       <c r="N19" s="8"/>
       <c r="O19" s="9"/>
       <c r="P19" s="8">
@@ -6316,13 +6395,13 @@
       </c>
       <c r="Q19" s="9"/>
       <c r="R19" s="8">
-        <v>3000000.0</v>
+        <v>1636927.0</v>
       </c>
       <c r="S19" s="8">
         <v>3000000.0</v>
       </c>
       <c r="T19" s="8">
-        <v>3000000.0</v>
+        <v>1583123.0</v>
       </c>
       <c r="U19" s="8">
         <v>750000.0</v>
@@ -6331,13 +6410,13 @@
         <v>0.25</v>
       </c>
       <c r="W19" s="8">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X19" s="9">
         <v>0.01</v>
       </c>
       <c r="Y19" s="8">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z19" s="9"/>
       <c r="AA19" s="8">
@@ -6377,11 +6456,21 @@
         <v>0.0</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="I20" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K20" s="1">
+        <v>13631.0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>69492.0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1293581.0</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="2"/>
       <c r="P20" s="6">
@@ -6389,13 +6478,13 @@
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="1">
-        <v>3000000.0</v>
+        <v>1706419.0</v>
       </c>
       <c r="S20" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T20" s="1">
-        <v>3000000.0</v>
+        <v>1666246.0</v>
       </c>
       <c r="U20" s="6">
         <v>750000.0</v>
@@ -6404,13 +6493,13 @@
         <v>0.25</v>
       </c>
       <c r="W20" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X20" s="2">
         <v>0.01</v>
       </c>
       <c r="Y20" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
@@ -6449,11 +6538,21 @@
         <v>0.0</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="I21" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K21" s="1">
+        <v>12936.0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>70187.0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1223393.0</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="2"/>
       <c r="P21" s="6">
@@ -6461,13 +6560,13 @@
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="1">
-        <v>3000000.0</v>
+        <v>1776607.0</v>
       </c>
       <c r="S21" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T21" s="1">
-        <v>3000000.0</v>
+        <v>1749369.0</v>
       </c>
       <c r="U21" s="6">
         <v>750000.0</v>
@@ -6476,13 +6575,13 @@
         <v>0.25</v>
       </c>
       <c r="W21" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X21" s="2">
         <v>0.01</v>
       </c>
       <c r="Y21" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="1">
@@ -6521,11 +6620,21 @@
         <v>0.0</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="I22" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K22" s="1">
+        <v>12234.0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>70889.0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1152504.0</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="2"/>
       <c r="P22" s="6">
@@ -6533,13 +6642,13 @@
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="1">
-        <v>3000000.0</v>
+        <v>1847496.0</v>
       </c>
       <c r="S22" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T22" s="1">
-        <v>3000000.0</v>
+        <v>1832492.0</v>
       </c>
       <c r="U22" s="6">
         <v>750000.0</v>
@@ -6548,13 +6657,13 @@
         <v>0.25</v>
       </c>
       <c r="W22" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X22" s="2">
         <v>0.01</v>
       </c>
       <c r="Y22" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="1">
@@ -6593,11 +6702,21 @@
         <v>0.0</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="I23" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K23" s="1">
+        <v>11525.0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>71598.0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1080906.0</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="2"/>
       <c r="P23" s="6">
@@ -6605,13 +6724,13 @@
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="1">
-        <v>3000000.0</v>
+        <v>1919094.0</v>
       </c>
       <c r="S23" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T23" s="1">
-        <v>3000000.0</v>
+        <v>1915615.0</v>
       </c>
       <c r="U23" s="6">
         <v>750000.0</v>
@@ -6620,13 +6739,13 @@
         <v>0.25</v>
       </c>
       <c r="W23" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X23" s="2">
         <v>0.01</v>
       </c>
       <c r="Y23" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="1">
@@ -6665,11 +6784,21 @@
         <v>0.0</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="I24" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K24" s="1">
+        <v>10809.0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>72314.0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1008593.0</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="2"/>
       <c r="P24" s="6">
@@ -6677,13 +6806,13 @@
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="1">
-        <v>3000000.0</v>
+        <v>1991407.0</v>
       </c>
       <c r="S24" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T24" s="1">
-        <v>3000000.0</v>
+        <v>1998738.0</v>
       </c>
       <c r="U24" s="6">
         <v>750000.0</v>
@@ -6692,13 +6821,13 @@
         <v>0.25</v>
       </c>
       <c r="W24" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X24" s="2">
         <v>0.01</v>
       </c>
       <c r="Y24" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="1">
@@ -6737,11 +6866,21 @@
         <v>0.0</v>
       </c>
       <c r="H25" s="2"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="I25" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K25" s="1">
+        <v>10086.0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>73037.0</v>
+      </c>
+      <c r="M25" s="1">
+        <v>935555.0</v>
+      </c>
       <c r="N25" s="1"/>
       <c r="O25" s="2"/>
       <c r="P25" s="6">
@@ -6749,13 +6888,13 @@
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="1">
-        <v>3000000.0</v>
+        <v>2064445.0</v>
       </c>
       <c r="S25" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T25" s="1">
-        <v>3000000.0</v>
+        <v>2081861.0</v>
       </c>
       <c r="U25" s="6">
         <v>750000.0</v>
@@ -6764,13 +6903,13 @@
         <v>0.25</v>
       </c>
       <c r="W25" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X25" s="2">
         <v>0.01</v>
       </c>
       <c r="Y25" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z25" s="2"/>
       <c r="AA25" s="1">
@@ -6809,11 +6948,21 @@
         <v>0.0</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="I26" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K26" s="1">
+        <v>9356.0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>73767.0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>861788.0</v>
+      </c>
       <c r="N26" s="1"/>
       <c r="O26" s="2"/>
       <c r="P26" s="6">
@@ -6821,13 +6970,13 @@
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="1">
-        <v>3000000.0</v>
+        <v>2138212.0</v>
       </c>
       <c r="S26" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T26" s="1">
-        <v>3000000.0</v>
+        <v>2164984.0</v>
       </c>
       <c r="U26" s="6">
         <v>750000.0</v>
@@ -6836,13 +6985,13 @@
         <v>0.25</v>
       </c>
       <c r="W26" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X26" s="2">
         <v>0.01</v>
       </c>
       <c r="Y26" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="1">
@@ -6881,11 +7030,21 @@
         <v>0.0</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="I27" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K27" s="1">
+        <v>8618.0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>74505.0</v>
+      </c>
+      <c r="M27" s="1">
+        <v>787283.0</v>
+      </c>
       <c r="N27" s="1"/>
       <c r="O27" s="2"/>
       <c r="P27" s="6">
@@ -6893,13 +7052,13 @@
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="1">
-        <v>3000000.0</v>
+        <v>2212717.0</v>
       </c>
       <c r="S27" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T27" s="1">
-        <v>3000000.0</v>
+        <v>2248107.0</v>
       </c>
       <c r="U27" s="6">
         <v>750000.0</v>
@@ -6908,13 +7067,13 @@
         <v>0.25</v>
       </c>
       <c r="W27" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X27" s="2">
         <v>0.01</v>
       </c>
       <c r="Y27" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="1">
@@ -6953,11 +7112,21 @@
         <v>0.0</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="I28" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K28" s="1">
+        <v>7873.0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>75250.0</v>
+      </c>
+      <c r="M28" s="1">
+        <v>712033.0</v>
+      </c>
       <c r="N28" s="1"/>
       <c r="O28" s="2"/>
       <c r="P28" s="6">
@@ -6965,13 +7134,13 @@
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="1">
-        <v>3000000.0</v>
+        <v>2287967.0</v>
       </c>
       <c r="S28" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T28" s="1">
-        <v>3000000.0</v>
+        <v>2331230.0</v>
       </c>
       <c r="U28" s="6">
         <v>750000.0</v>
@@ -6980,13 +7149,13 @@
         <v>0.25</v>
       </c>
       <c r="W28" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X28" s="2">
         <v>0.01</v>
       </c>
       <c r="Y28" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="1">
@@ -7025,11 +7194,21 @@
         <v>0.0</v>
       </c>
       <c r="H29" s="2"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="I29" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K29" s="1">
+        <v>7120.0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>76003.0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>636030.0</v>
+      </c>
       <c r="N29" s="1"/>
       <c r="O29" s="2"/>
       <c r="P29" s="6">
@@ -7037,13 +7216,13 @@
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="1">
-        <v>3000000.0</v>
+        <v>2363970.0</v>
       </c>
       <c r="S29" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T29" s="1">
-        <v>3000000.0</v>
+        <v>2414353.0</v>
       </c>
       <c r="U29" s="6">
         <v>750000.0</v>
@@ -7052,13 +7231,13 @@
         <v>0.25</v>
       </c>
       <c r="W29" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X29" s="2">
         <v>0.01</v>
       </c>
       <c r="Y29" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="1">
@@ -7097,11 +7276,21 @@
         <v>0.0</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="I30" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K30" s="1">
+        <v>6360.0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>76763.0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>559268.0</v>
+      </c>
       <c r="N30" s="1"/>
       <c r="O30" s="2"/>
       <c r="P30" s="6">
@@ -7109,13 +7298,13 @@
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="1">
-        <v>3000000.0</v>
+        <v>2440732.0</v>
       </c>
       <c r="S30" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T30" s="1">
-        <v>3000000.0</v>
+        <v>2497476.0</v>
       </c>
       <c r="U30" s="6">
         <v>750000.0</v>
@@ -7124,13 +7313,13 @@
         <v>0.25</v>
       </c>
       <c r="W30" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X30" s="2">
         <v>0.01</v>
       </c>
       <c r="Y30" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="1">
@@ -7169,11 +7358,21 @@
         <v>0.0</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
+      <c r="I31" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K31" s="1">
+        <v>5593.0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>77530.0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>481737.0</v>
+      </c>
       <c r="N31" s="1"/>
       <c r="O31" s="2"/>
       <c r="P31" s="6">
@@ -7181,13 +7380,13 @@
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="1">
-        <v>3000000.0</v>
+        <v>2518263.0</v>
       </c>
       <c r="S31" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T31" s="1">
-        <v>3000000.0</v>
+        <v>2580599.0</v>
       </c>
       <c r="U31" s="6">
         <v>750000.0</v>
@@ -7196,13 +7395,13 @@
         <v>0.25</v>
       </c>
       <c r="W31" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X31" s="2">
         <v>0.01</v>
       </c>
       <c r="Y31" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="1">
@@ -7241,11 +7440,21 @@
         <v>0.0</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+      <c r="I32" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K32" s="1">
+        <v>4817.0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>78306.0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>403432.0</v>
+      </c>
       <c r="N32" s="1"/>
       <c r="O32" s="2"/>
       <c r="P32" s="6">
@@ -7253,13 +7462,13 @@
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="1">
-        <v>3000000.0</v>
+        <v>2596568.0</v>
       </c>
       <c r="S32" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T32" s="1">
-        <v>3000000.0</v>
+        <v>2663722.0</v>
       </c>
       <c r="U32" s="6">
         <v>750000.0</v>
@@ -7268,13 +7477,13 @@
         <v>0.25</v>
       </c>
       <c r="W32" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X32" s="2">
         <v>0.01</v>
       </c>
       <c r="Y32" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="1">
@@ -7313,11 +7522,21 @@
         <v>0.0</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="I33" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K33" s="1">
+        <v>4034.0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>79089.0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>324343.0</v>
+      </c>
       <c r="N33" s="1"/>
       <c r="O33" s="2"/>
       <c r="P33" s="6">
@@ -7325,13 +7544,13 @@
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="1">
-        <v>3000000.0</v>
+        <v>2675657.0</v>
       </c>
       <c r="S33" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T33" s="1">
-        <v>3000000.0</v>
+        <v>2746845.0</v>
       </c>
       <c r="U33" s="6">
         <v>750000.0</v>
@@ -7340,13 +7559,13 @@
         <v>0.25</v>
       </c>
       <c r="W33" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X33" s="2">
         <v>0.01</v>
       </c>
       <c r="Y33" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z33" s="2"/>
       <c r="AA33" s="1">
@@ -7385,11 +7604,21 @@
         <v>0.0</v>
       </c>
       <c r="H34" s="2"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="I34" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K34" s="1">
+        <v>3243.0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>79880.0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>244463.0</v>
+      </c>
       <c r="N34" s="1"/>
       <c r="O34" s="2"/>
       <c r="P34" s="6">
@@ -7397,13 +7626,13 @@
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="1">
-        <v>3000000.0</v>
+        <v>2755537.0</v>
       </c>
       <c r="S34" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T34" s="1">
-        <v>3000000.0</v>
+        <v>2829968.0</v>
       </c>
       <c r="U34" s="6">
         <v>750000.0</v>
@@ -7412,13 +7641,13 @@
         <v>0.25</v>
       </c>
       <c r="W34" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X34" s="2">
         <v>0.01</v>
       </c>
       <c r="Y34" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="1">
@@ -7457,11 +7686,21 @@
         <v>0.0</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
+      <c r="I35" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K35" s="1">
+        <v>2445.0</v>
+      </c>
+      <c r="L35" s="1">
+        <v>80678.0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>163785.0</v>
+      </c>
       <c r="N35" s="1"/>
       <c r="O35" s="2"/>
       <c r="P35" s="6">
@@ -7469,13 +7708,13 @@
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="1">
-        <v>3000000.0</v>
+        <v>2836215.0</v>
       </c>
       <c r="S35" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T35" s="1">
-        <v>3000000.0</v>
+        <v>2913091.0</v>
       </c>
       <c r="U35" s="6">
         <v>750000.0</v>
@@ -7484,13 +7723,13 @@
         <v>0.25</v>
       </c>
       <c r="W35" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X35" s="2">
         <v>0.01</v>
       </c>
       <c r="Y35" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="1">
@@ -7529,11 +7768,21 @@
         <v>0.0</v>
       </c>
       <c r="H36" s="2"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
+      <c r="I36" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1638.0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>81485.0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>82300.0</v>
+      </c>
       <c r="N36" s="1"/>
       <c r="O36" s="2"/>
       <c r="P36" s="6">
@@ -7541,13 +7790,13 @@
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="1">
-        <v>3000000.0</v>
+        <v>2917700.0</v>
       </c>
       <c r="S36" s="1">
         <v>3000000.0</v>
       </c>
       <c r="T36" s="1">
-        <v>3000000.0</v>
+        <v>2996214.0</v>
       </c>
       <c r="U36" s="6">
         <v>750000.0</v>
@@ -7556,13 +7805,13 @@
         <v>0.25</v>
       </c>
       <c r="W36" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X36" s="2">
         <v>0.01</v>
       </c>
       <c r="Y36" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="1">
@@ -7601,11 +7850,21 @@
         <v>0.0</v>
       </c>
       <c r="H37" s="2"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+      <c r="I37" s="1">
+        <v>83123.0</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K37" s="1">
+        <v>823.0</v>
+      </c>
+      <c r="L37" s="1">
+        <v>82300.0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0.0</v>
+      </c>
       <c r="N37" s="1"/>
       <c r="O37" s="2"/>
       <c r="P37" s="6">
@@ -7619,7 +7878,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T37" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U37" s="6">
         <v>750000.0</v>
@@ -7628,13 +7887,13 @@
         <v>0.25</v>
       </c>
       <c r="W37" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X37" s="2">
         <v>0.01</v>
       </c>
       <c r="Y37" s="1">
-        <v>-87600.0</v>
+        <v>-170723.0</v>
       </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="1">
@@ -7691,7 +7950,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T38" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U38" s="6">
         <v>750000.0</v>
@@ -7700,7 +7959,7 @@
         <v>0.25</v>
       </c>
       <c r="W38" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X38" s="2">
         <v>0.01</v>
@@ -7763,7 +8022,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T39" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U39" s="6">
         <v>750000.0</v>
@@ -7772,7 +8031,7 @@
         <v>0.25</v>
       </c>
       <c r="W39" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X39" s="2">
         <v>0.01</v>
@@ -7835,7 +8094,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T40" s="11">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U40" s="11">
         <v>750000.0</v>
@@ -7844,7 +8103,7 @@
         <v>0.25</v>
       </c>
       <c r="W40" s="11">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X40" s="12">
         <v>0.01</v>
@@ -7908,7 +8167,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T41" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U41" s="6">
         <v>750000.0</v>
@@ -7917,7 +8176,7 @@
         <v>0.25</v>
       </c>
       <c r="W41" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X41" s="2">
         <v>0.01</v>
@@ -7980,7 +8239,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T42" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U42" s="6">
         <v>750000.0</v>
@@ -7989,7 +8248,7 @@
         <v>0.25</v>
       </c>
       <c r="W42" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X42" s="2">
         <v>0.01</v>
@@ -8052,7 +8311,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T43" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U43" s="6">
         <v>750000.0</v>
@@ -8061,7 +8320,7 @@
         <v>0.25</v>
       </c>
       <c r="W43" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X43" s="2">
         <v>0.01</v>
@@ -8124,7 +8383,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T44" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U44" s="6">
         <v>750000.0</v>
@@ -8133,7 +8392,7 @@
         <v>0.25</v>
       </c>
       <c r="W44" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X44" s="2">
         <v>0.01</v>
@@ -8196,7 +8455,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T45" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U45" s="6">
         <v>750000.0</v>
@@ -8205,7 +8464,7 @@
         <v>0.25</v>
       </c>
       <c r="W45" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X45" s="2">
         <v>0.01</v>
@@ -8268,7 +8527,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T46" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U46" s="6">
         <v>750000.0</v>
@@ -8277,7 +8536,7 @@
         <v>0.25</v>
       </c>
       <c r="W46" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X46" s="2">
         <v>0.01</v>
@@ -8340,7 +8599,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T47" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U47" s="6">
         <v>750000.0</v>
@@ -8349,7 +8608,7 @@
         <v>0.25</v>
       </c>
       <c r="W47" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X47" s="2">
         <v>0.01</v>
@@ -8412,7 +8671,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T48" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U48" s="6">
         <v>750000.0</v>
@@ -8421,7 +8680,7 @@
         <v>0.25</v>
       </c>
       <c r="W48" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X48" s="2">
         <v>0.01</v>
@@ -8484,7 +8743,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T49" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U49" s="6">
         <v>750000.0</v>
@@ -8493,7 +8752,7 @@
         <v>0.25</v>
       </c>
       <c r="W49" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X49" s="2">
         <v>0.01</v>
@@ -8556,7 +8815,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T50" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U50" s="6">
         <v>750000.0</v>
@@ -8565,7 +8824,7 @@
         <v>0.25</v>
       </c>
       <c r="W50" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X50" s="2">
         <v>0.01</v>
@@ -8628,7 +8887,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T51" s="1">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U51" s="6">
         <v>750000.0</v>
@@ -8637,7 +8896,7 @@
         <v>0.25</v>
       </c>
       <c r="W51" s="1">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X51" s="2">
         <v>0.01</v>
@@ -8700,7 +8959,7 @@
         <v>3000000.0</v>
       </c>
       <c r="T52" s="5">
-        <v>3000000.0</v>
+        <v>3079337.0</v>
       </c>
       <c r="U52" s="5">
         <v>750000.0</v>
@@ -8709,7 +8968,7 @@
         <v>0.25</v>
       </c>
       <c r="W52" s="5">
-        <v>7500.0</v>
+        <v>0</v>
       </c>
       <c r="X52" s="16">
         <v>0.01</v>

</xml_diff>